<commit_message>
Deleted files as required
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/Taxonomy.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/Taxonomy.xlsx
@@ -50,7 +50,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="12">
+  <numFmts count="17">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>

</xml_diff>